<commit_message>
nomes normalizados e coluna de graduação removida
</commit_message>
<xml_diff>
--- a/T2/datasets/IO/CCR.xlsx
+++ b/T2/datasets/IO/CCR.xlsx
@@ -483,7 +483,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -516,7 +516,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -549,7 +549,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -582,7 +582,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -615,7 +615,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -648,7 +648,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -681,7 +681,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -714,7 +714,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -747,7 +747,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -780,7 +780,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -813,7 +813,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -846,7 +846,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -879,7 +879,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -912,7 +912,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -945,7 +945,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -978,7 +978,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1044,7 +1044,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1077,7 +1077,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1110,7 +1110,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1143,7 +1143,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1176,7 +1176,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1204,12 +1204,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Curso Superior de Tecnologia em Agronegócio</t>
+          <t>Curso Superior de Tecnologia em Agronegocio</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1237,12 +1237,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Curso Superior de Tecnologia em Agronegócio</t>
+          <t>Curso Superior de Tecnologia em Agronegocio</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1270,12 +1270,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Curso Superior de Tecnologia em Agronegócio</t>
+          <t>Curso Superior de Tecnologia em Agronegocio</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1303,12 +1303,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Curso Superior de Tecnologia em Agronegócio</t>
+          <t>Curso Superior de Tecnologia em Agronegocio</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1336,12 +1336,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Curso Superior de Tecnologia em Agronegócio</t>
+          <t>Curso Superior de Tecnologia em Agronegocio</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1369,12 +1369,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Curso Superior de Tecnologia em Agronegócio</t>
+          <t>Curso Superior de Tecnologia em Agronegocio</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1402,12 +1402,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Curso Superior de Tecnologia em Agronegócio</t>
+          <t>Curso Superior de Tecnologia em Agronegocio</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1435,12 +1435,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Curso Superior de Tecnologia em Agronegócio</t>
+          <t>Curso Superior de Tecnologia em Agronegocio</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1468,12 +1468,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Curso Superior de Tecnologia em Agronegócio</t>
+          <t>Curso Superior de Tecnologia em Agronegocio</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1501,12 +1501,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Curso Superior de Tecnologia em Agronegócio</t>
+          <t>Curso Superior de Tecnologia em Agronegocio</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1534,12 +1534,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Curso Superior de Tecnologia em Agronegócio</t>
+          <t>Curso Superior de Tecnologia em Agronegocio</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1567,12 +1567,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Curso Superior de Tecnologia em Agronegócio</t>
+          <t>Curso Superior de Tecnologia em Agronegocio</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1600,12 +1600,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Curso Superior de Tecnologia em Agronegócio</t>
+          <t>Curso Superior de Tecnologia em Agronegocio</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1633,12 +1633,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Curso Superior de Tecnologia em Agronegócio</t>
+          <t>Curso Superior de Tecnologia em Agronegocio</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1666,12 +1666,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Curso Superior de Tecnologia em Agronegócio</t>
+          <t>Curso Superior de Tecnologia em Agronegocio</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1699,12 +1699,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Curso Superior de Tecnologia em Agronegócio</t>
+          <t>Curso Superior de Tecnologia em Agronegocio</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1732,12 +1732,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Curso Superior de Tecnologia em Agronegócio</t>
+          <t>Curso Superior de Tecnologia em Agronegocio</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1765,12 +1765,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Curso Superior de Tecnologia em Agronegócio</t>
+          <t>Curso Superior de Tecnologia em Agronegocio</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1798,12 +1798,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Curso Superior de Tecnologia em Agronegócio</t>
+          <t>Curso Superior de Tecnologia em Agronegocio</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1831,12 +1831,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Curso Superior de Tecnologia em Agronegócio</t>
+          <t>Curso Superior de Tecnologia em Agronegocio</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1864,12 +1864,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Curso Superior de Tecnologia em Agronegócio</t>
+          <t>Curso Superior de Tecnologia em Agronegocio</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1897,12 +1897,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Curso Superior de Tecnologia em Agronegócio</t>
+          <t>Curso Superior de Tecnologia em Agronegocio</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1935,7 +1935,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1968,7 +1968,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -2001,7 +2001,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -2034,7 +2034,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -2067,7 +2067,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -2100,7 +2100,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -2133,7 +2133,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -2166,7 +2166,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2199,7 +2199,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -2232,7 +2232,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -2265,7 +2265,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2298,7 +2298,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -2331,7 +2331,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -2364,7 +2364,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -2397,7 +2397,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2430,7 +2430,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2463,7 +2463,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2496,7 +2496,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2529,7 +2529,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2595,7 +2595,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2628,7 +2628,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2661,7 +2661,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2694,7 +2694,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2727,7 +2727,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2760,7 +2760,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2793,7 +2793,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2826,7 +2826,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2859,7 +2859,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2892,7 +2892,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2925,7 +2925,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2958,7 +2958,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2991,7 +2991,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -3024,7 +3024,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -3057,7 +3057,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -3090,7 +3090,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -3123,7 +3123,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -3156,7 +3156,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -3189,7 +3189,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -3222,7 +3222,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -3255,7 +3255,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -3288,7 +3288,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -3321,7 +3321,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -3354,7 +3354,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -3382,12 +3382,12 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Agudo/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Agudo/RS</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -3415,12 +3415,12 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Agudo/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Agudo/RS</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -3448,12 +3448,12 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Agudo/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Agudo/RS</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -3481,12 +3481,12 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Agudo/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Agudo/RS</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -3514,12 +3514,12 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Agudo/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Agudo/RS</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -3547,12 +3547,12 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Agudo/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Agudo/RS</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -3580,12 +3580,12 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Agudo/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Agudo/RS</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -3613,12 +3613,12 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Agudo/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Agudo/RS</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -3646,12 +3646,12 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Agudo/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Agudo/RS</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -3679,12 +3679,12 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Agudo/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Agudo/RS</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -3712,12 +3712,12 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Balneário Pinhal/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Balneario Pinhal/RS</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -3745,12 +3745,12 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Balneário Pinhal/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Balneario Pinhal/RS</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -3778,12 +3778,12 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Balneário Pinhal/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Balneario Pinhal/RS</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -3811,12 +3811,12 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Balneário Pinhal/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Balneario Pinhal/RS</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -3844,12 +3844,12 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Balneário Pinhal/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Balneario Pinhal/RS</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3877,12 +3877,12 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Balneário Pinhal/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Balneario Pinhal/RS</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3910,12 +3910,12 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Canguçu/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Cangucu/RS</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3943,12 +3943,12 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Canguçu/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Cangucu/RS</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3976,12 +3976,12 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Canguçu/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Cangucu/RS</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -4009,12 +4009,12 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Canguçu/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Cangucu/RS</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -4042,12 +4042,12 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Cerro Largo/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Cerro Largo/RS</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -4075,12 +4075,12 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Cerro Largo/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Cerro Largo/RS</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -4108,12 +4108,12 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Cerro Largo/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Cerro Largo/RS</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -4141,12 +4141,12 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Cerro Largo/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Cerro Largo/RS</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -4174,12 +4174,12 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Cerro Largo/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Cerro Largo/RS</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -4207,12 +4207,12 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Cerro Largo/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Cerro Largo/RS</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -4240,12 +4240,12 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Cerro Largo/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Cerro Largo/RS</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -4273,12 +4273,12 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Cerro Largo/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Cerro Largo/RS</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -4306,12 +4306,12 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Cerro Largo/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Cerro Largo/RS</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -4339,12 +4339,12 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Encantado/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Encantado/RS</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -4372,12 +4372,12 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Encantado/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Encantado/RS</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -4405,12 +4405,12 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Encantado/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Encantado/RS</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -4438,12 +4438,12 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Encantado/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Encantado/RS</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -4471,12 +4471,12 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Encantado/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Encantado/RS</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -4504,12 +4504,12 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Encantado/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Encantado/RS</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -4537,12 +4537,12 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Encantado/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Encantado/RS</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -4570,12 +4570,12 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Itaqui/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Itaqui/RS</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -4603,12 +4603,12 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Itaqui/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Itaqui/RS</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -4636,12 +4636,12 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Itaqui/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Itaqui/RS</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -4669,12 +4669,12 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Itaqui/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Itaqui/RS</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -4702,12 +4702,12 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Itaqui/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Itaqui/RS</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -4735,12 +4735,12 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Itaqui/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Itaqui/RS</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -4768,12 +4768,12 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Itaqui/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Itaqui/RS</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -4801,12 +4801,12 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Itaqui/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Itaqui/RS</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -4834,12 +4834,12 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Itaqui/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Itaqui/RS</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -4867,12 +4867,12 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Novo Hamburgo/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Novo Hamburgo/RS</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -4900,12 +4900,12 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Novo Hamburgo/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Novo Hamburgo/RS</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -4933,12 +4933,12 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Novo Hamburgo/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Novo Hamburgo/RS</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -4966,12 +4966,12 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Novo Hamburgo/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Novo Hamburgo/RS</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -4999,12 +4999,12 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Novo Hamburgo/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Novo Hamburgo/RS</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -5032,12 +5032,12 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Novo Hamburgo/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Novo Hamburgo/RS</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -5065,12 +5065,12 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Santana do Livramento/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Santana do Livramento/RS</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -5098,12 +5098,12 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Santana do Livramento/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Santana do Livramento/RS</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -5131,12 +5131,12 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Santana do Livramento/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Santana do Livramento/RS</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -5164,12 +5164,12 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Santana do Livramento/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Santana do Livramento/RS</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -5197,12 +5197,12 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Santana do Livramento/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Santana do Livramento/RS</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -5230,12 +5230,12 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Santana do Livramento/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Santana do Livramento/RS</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -5263,12 +5263,12 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Santana do Livramento/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Santana do Livramento/RS</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -5296,12 +5296,12 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Santiago/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Santiago/RS</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -5329,12 +5329,12 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Santiago/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Santiago/RS</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -5362,12 +5362,12 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Santiago/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Santiago/RS</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -5395,12 +5395,12 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Santiago/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Santiago/RS</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
@@ -5428,12 +5428,12 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/São Gabriel/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Sao Gabriel/RS</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -5461,12 +5461,12 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/São Gabriel/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Sao Gabriel/RS</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
@@ -5494,12 +5494,12 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/São Gabriel/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Sao Gabriel/RS</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
@@ -5527,12 +5527,12 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/São Gabriel/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Sao Gabriel/RS</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
@@ -5560,12 +5560,12 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/São Lourenço do Sul/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Sao Lourenco do Sul/RS</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
@@ -5593,12 +5593,12 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/São Lourenço do Sul/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Sao Lourenco do Sul/RS</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
@@ -5626,12 +5626,12 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/São Lourenço do Sul/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Sao Lourenco do Sul/RS</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
@@ -5659,12 +5659,12 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/São Lourenço do Sul/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Sao Lourenco do Sul/RS</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
@@ -5692,12 +5692,12 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/São Lourenço do Sul/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Sao Lourenco do Sul/RS</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
@@ -5725,12 +5725,12 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/São Lourenço do Sul/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Sao Lourenco do Sul/RS</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
@@ -5758,12 +5758,12 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/São Sepé/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Sao Sepe/RS</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
@@ -5791,12 +5791,12 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/São Sepé/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Sao Sepe/RS</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
@@ -5824,12 +5824,12 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/São Sepé/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Sao Sepe/RS</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
@@ -5857,12 +5857,12 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/São Sepé/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Sao Sepe/RS</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
@@ -5890,12 +5890,12 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/São Sepé/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Sao Sepe/RS</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
@@ -5923,12 +5923,12 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/São Sepé/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Sao Sepe/RS</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
@@ -5956,12 +5956,12 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/São Sepé/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Sao Sepe/RS</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
@@ -5989,12 +5989,12 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/São Sepé/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Sao Sepe/RS</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
@@ -6022,12 +6022,12 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Seberi/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Seberi/RS</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
@@ -6055,12 +6055,12 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Seberi/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Seberi/RS</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
@@ -6088,12 +6088,12 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Seberi/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Seberi/RS</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
@@ -6121,12 +6121,12 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Seberi/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Seberi/RS</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
@@ -6154,12 +6154,12 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Seberi/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Seberi/RS</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
@@ -6187,12 +6187,12 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Seberi/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Seberi/RS</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
@@ -6220,12 +6220,12 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Seberi/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Seberi/RS</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
@@ -6253,12 +6253,12 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Seberi/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Seberi/RS</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
@@ -6286,12 +6286,12 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Seberi/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Seberi/RS</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
@@ -6319,12 +6319,12 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Serafina Corrêa/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Serafina Correa/RS</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
@@ -6352,12 +6352,12 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Serafina Corrêa/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Serafina Correa/RS</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
@@ -6385,12 +6385,12 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Serafina Corrêa/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Serafina Correa/RS</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
@@ -6418,12 +6418,12 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Serafina Corrêa/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Serafina Correa/RS</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D182" t="inlineStr">
@@ -6451,12 +6451,12 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Sobradinho/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Sobradinho/RS</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D183" t="inlineStr">
@@ -6484,12 +6484,12 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Sobradinho/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Sobradinho/RS</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
@@ -6517,12 +6517,12 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Sobradinho/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Sobradinho/RS</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D185" t="inlineStr">
@@ -6550,12 +6550,12 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Sobradinho/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Sobradinho/RS</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
@@ -6583,12 +6583,12 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Sobradinho/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Sobradinho/RS</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
@@ -6616,12 +6616,12 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Sobradinho/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Sobradinho/RS</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
@@ -6649,12 +6649,12 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Três de Maio/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Tres de Maio/RS</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
@@ -6682,12 +6682,12 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Três de Maio/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Tres de Maio/RS</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
@@ -6715,12 +6715,12 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Três de Maio/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Tres de Maio/RS</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
@@ -6748,12 +6748,12 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Licenciatura em Educação do Campo/Distância/Três de Maio/RS</t>
+          <t>Licenciatura em Educacao do Campo/Distancia/Tres de Maio/RS</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
@@ -6781,12 +6781,12 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Medicina Veterinária</t>
+          <t>Medicina Veterinaria</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
@@ -6814,12 +6814,12 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Medicina Veterinária</t>
+          <t>Medicina Veterinaria</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
@@ -6847,12 +6847,12 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Medicina Veterinária</t>
+          <t>Medicina Veterinaria</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D195" t="inlineStr">
@@ -6880,12 +6880,12 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Medicina Veterinária</t>
+          <t>Medicina Veterinaria</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D196" t="inlineStr">
@@ -6913,12 +6913,12 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Medicina Veterinária</t>
+          <t>Medicina Veterinaria</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D197" t="inlineStr">
@@ -6946,12 +6946,12 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Medicina Veterinária</t>
+          <t>Medicina Veterinaria</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
@@ -6979,12 +6979,12 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Medicina Veterinária</t>
+          <t>Medicina Veterinaria</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
@@ -7012,12 +7012,12 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Medicina Veterinária</t>
+          <t>Medicina Veterinaria</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
@@ -7045,12 +7045,12 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Medicina Veterinária</t>
+          <t>Medicina Veterinaria</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
@@ -7078,12 +7078,12 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Medicina Veterinária</t>
+          <t>Medicina Veterinaria</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D202" t="inlineStr">
@@ -7111,12 +7111,12 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Medicina Veterinária</t>
+          <t>Medicina Veterinaria</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D203" t="inlineStr">
@@ -7144,12 +7144,12 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Medicina Veterinária</t>
+          <t>Medicina Veterinaria</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D204" t="inlineStr">
@@ -7177,12 +7177,12 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Medicina Veterinária</t>
+          <t>Medicina Veterinaria</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D205" t="inlineStr">
@@ -7210,12 +7210,12 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Medicina Veterinária</t>
+          <t>Medicina Veterinaria</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D206" t="inlineStr">
@@ -7243,12 +7243,12 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Medicina Veterinária</t>
+          <t>Medicina Veterinaria</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D207" t="inlineStr">
@@ -7276,12 +7276,12 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Medicina Veterinária</t>
+          <t>Medicina Veterinaria</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D208" t="inlineStr">
@@ -7309,12 +7309,12 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Medicina Veterinária</t>
+          <t>Medicina Veterinaria</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D209" t="inlineStr">
@@ -7342,12 +7342,12 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Medicina Veterinária</t>
+          <t>Medicina Veterinaria</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D210" t="inlineStr">
@@ -7375,12 +7375,12 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Medicina Veterinária</t>
+          <t>Medicina Veterinaria</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D211" t="inlineStr">
@@ -7408,12 +7408,12 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Medicina Veterinária</t>
+          <t>Medicina Veterinaria</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D212" t="inlineStr">
@@ -7441,12 +7441,12 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Medicina Veterinária</t>
+          <t>Medicina Veterinaria</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D213" t="inlineStr">
@@ -7474,12 +7474,12 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Medicina Veterinária</t>
+          <t>Medicina Veterinaria</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D214" t="inlineStr">
@@ -7507,12 +7507,12 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Faxinal do Soturno/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Faxinal do Soturno/RS</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D215" t="inlineStr">
@@ -7540,12 +7540,12 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Faxinal do Soturno/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Faxinal do Soturno/RS</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D216" t="inlineStr">
@@ -7573,12 +7573,12 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Faxinal do Soturno/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Faxinal do Soturno/RS</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D217" t="inlineStr">
@@ -7606,12 +7606,12 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Faxinal do Soturno/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Faxinal do Soturno/RS</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D218" t="inlineStr">
@@ -7639,12 +7639,12 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Faxinal do Soturno/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Faxinal do Soturno/RS</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D219" t="inlineStr">
@@ -7672,12 +7672,12 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Faxinal do Soturno/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Faxinal do Soturno/RS</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D220" t="inlineStr">
@@ -7705,12 +7705,12 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Faxinal do Soturno/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Faxinal do Soturno/RS</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D221" t="inlineStr">
@@ -7738,12 +7738,12 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Faxinal do Soturno/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Faxinal do Soturno/RS</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D222" t="inlineStr">
@@ -7771,12 +7771,12 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Faxinal do Soturno/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Faxinal do Soturno/RS</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D223" t="inlineStr">
@@ -7804,12 +7804,12 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Quaraí/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Quarai/RS</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D224" t="inlineStr">
@@ -7837,12 +7837,12 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Quaraí/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Quarai/RS</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D225" t="inlineStr">
@@ -7870,12 +7870,12 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Quaraí/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Quarai/RS</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D226" t="inlineStr">
@@ -7903,12 +7903,12 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Quaraí/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Quarai/RS</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D227" t="inlineStr">
@@ -7936,12 +7936,12 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Quaraí/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Quarai/RS</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D228" t="inlineStr">
@@ -7969,12 +7969,12 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Sarandi/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Sarandi/RS</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D229" t="inlineStr">
@@ -8002,12 +8002,12 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Sarandi/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Sarandi/RS</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D230" t="inlineStr">
@@ -8035,12 +8035,12 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Sarandi/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Sarandi/RS</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D231" t="inlineStr">
@@ -8068,12 +8068,12 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Sarandi/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Sarandi/RS</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D232" t="inlineStr">
@@ -8101,12 +8101,12 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Sarandi/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Sarandi/RS</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D233" t="inlineStr">
@@ -8134,12 +8134,12 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Sarandi/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Sarandi/RS</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D234" t="inlineStr">
@@ -8167,12 +8167,12 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Sobradinho/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Sobradinho/RS</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D235" t="inlineStr">
@@ -8200,12 +8200,12 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Sobradinho/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Sobradinho/RS</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D236" t="inlineStr">
@@ -8233,12 +8233,12 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Sobradinho/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Sobradinho/RS</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D237" t="inlineStr">
@@ -8266,12 +8266,12 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Sobradinho/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Sobradinho/RS</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D238" t="inlineStr">
@@ -8299,12 +8299,12 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Sobradinho/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Sobradinho/RS</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D239" t="inlineStr">
@@ -8332,12 +8332,12 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Sobradinho/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Sobradinho/RS</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D240" t="inlineStr">
@@ -8365,12 +8365,12 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Sobradinho/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Sobradinho/RS</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D241" t="inlineStr">
@@ -8398,12 +8398,12 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Sobradinho/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Sobradinho/RS</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D242" t="inlineStr">
@@ -8431,12 +8431,12 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Três de Maio/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Tres de Maio/RS</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D243" t="inlineStr">
@@ -8464,12 +8464,12 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Três de Maio/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Tres de Maio/RS</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D244" t="inlineStr">
@@ -8497,12 +8497,12 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Três de Maio/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Tres de Maio/RS</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D245" t="inlineStr">
@@ -8530,12 +8530,12 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Três de Maio/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Tres de Maio/RS</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D246" t="inlineStr">
@@ -8563,12 +8563,12 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Três de Maio/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Tres de Maio/RS</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D247" t="inlineStr">
@@ -8596,12 +8596,12 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Três de Maio/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Tres de Maio/RS</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D248" t="inlineStr">
@@ -8629,12 +8629,12 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Três de Maio/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Tres de Maio/RS</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D249" t="inlineStr">
@@ -8662,12 +8662,12 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Três de Maio/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Tres de Maio/RS</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D250" t="inlineStr">
@@ -8695,12 +8695,12 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Vila Flores/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Vila Flores/RS</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D251" t="inlineStr">
@@ -8728,12 +8728,12 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Vila Flores/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Vila Flores/RS</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D252" t="inlineStr">
@@ -8761,12 +8761,12 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Vila Flores/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Vila Flores/RS</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D253" t="inlineStr">
@@ -8794,12 +8794,12 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Vila Flores/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Vila Flores/RS</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D254" t="inlineStr">
@@ -8827,12 +8827,12 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Vila Flores/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Vila Flores/RS</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D255" t="inlineStr">
@@ -8860,12 +8860,12 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Vila Flores/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Vila Flores/RS</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D256" t="inlineStr">
@@ -8893,12 +8893,12 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Tec. Agric. Familiar Sustentabilidade/Distância/Vila Flores/RS</t>
+          <t>Tec. Agric. Familiar Sustentabilidade/Distancia/Vila Flores/RS</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D257" t="inlineStr">
@@ -8931,7 +8931,7 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D258" t="inlineStr">
@@ -8964,7 +8964,7 @@
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D259" t="inlineStr">
@@ -8997,7 +8997,7 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D260" t="inlineStr">
@@ -9030,7 +9030,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D261" t="inlineStr">
@@ -9063,7 +9063,7 @@
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D262" t="inlineStr">
@@ -9096,7 +9096,7 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D263" t="inlineStr">
@@ -9129,7 +9129,7 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D264" t="inlineStr">
@@ -9162,7 +9162,7 @@
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D265" t="inlineStr">
@@ -9195,7 +9195,7 @@
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D266" t="inlineStr">
@@ -9228,7 +9228,7 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D267" t="inlineStr">
@@ -9261,7 +9261,7 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D268" t="inlineStr">
@@ -9294,7 +9294,7 @@
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D269" t="inlineStr">
@@ -9327,7 +9327,7 @@
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D270" t="inlineStr">
@@ -9360,7 +9360,7 @@
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D271" t="inlineStr">
@@ -9393,7 +9393,7 @@
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D272" t="inlineStr">
@@ -9426,7 +9426,7 @@
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D273" t="inlineStr">
@@ -9459,7 +9459,7 @@
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D274" t="inlineStr">
@@ -9492,7 +9492,7 @@
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D275" t="inlineStr">
@@ -9525,7 +9525,7 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D276" t="inlineStr">
@@ -9558,7 +9558,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D277" t="inlineStr">
@@ -9591,7 +9591,7 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D278" t="inlineStr">
@@ -9624,7 +9624,7 @@
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>Graduação</t>
+          <t>Graduacao</t>
         </is>
       </c>
       <c r="D279" t="inlineStr">

</xml_diff>